<commit_message>
added .yml file and pwertrains and segments parameters
</commit_message>
<xml_diff>
--- a/data/ODYM_Config_Al_cars.xlsx
+++ b/data/ODYM_Config_Al_cars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAE13EB-393C-420B-AC3B-4721B791C2D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450A66F5-852F-4194-BB50-4F3D4BB97AE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="844" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="160">
   <si>
     <t>Description</t>
   </si>
@@ -324,9 +324,6 @@
     <t>Powertrain_and_Segment</t>
   </si>
   <si>
-    <t>Powertrain and Marketing segment by cohor and region</t>
-  </si>
-  <si>
     <t>p</t>
   </si>
   <si>
@@ -493,6 +490,27 @@
   </si>
   <si>
     <t>Alloy sorting rate</t>
+  </si>
+  <si>
+    <t>Powertrains</t>
+  </si>
+  <si>
+    <t>Segments</t>
+  </si>
+  <si>
+    <t>Powertrain and Marketing segment by cohort and region</t>
+  </si>
+  <si>
+    <t>Powertrain split by cohort and region</t>
+  </si>
+  <si>
+    <t>Srpc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segment split by cohort and region </t>
+  </si>
+  <si>
+    <t>Srsc</t>
   </si>
 </sst>
 </file>
@@ -1237,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:K70"/>
+  <dimension ref="A2:K72"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B53" sqref="A53:XFD53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1574,7 +1592,7 @@
         <v>20</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I21" t="s">
         <v>92</v>
@@ -1597,79 +1615,79 @@
         <v>20</v>
       </c>
       <c r="H22" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C23" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E23" t="s">
         <v>91</v>
       </c>
       <c r="F23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G23" t="s">
         <v>20</v>
       </c>
       <c r="H23" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C24" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D24" s="38" t="s">
         <v>129</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>130</v>
       </c>
       <c r="E24" t="s">
         <v>91</v>
       </c>
       <c r="F24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G24" t="s">
         <v>20</v>
       </c>
       <c r="H24" s="26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C25" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="E25" t="s">
+        <v>141</v>
+      </c>
+      <c r="F25" t="s">
+        <v>141</v>
+      </c>
+      <c r="G25" t="s">
         <v>143</v>
       </c>
-      <c r="E25" t="s">
-        <v>142</v>
-      </c>
-      <c r="F25" t="s">
-        <v>142</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="H25" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="H25" s="26" t="s">
-        <v>145</v>
-      </c>
       <c r="I25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.3">
@@ -1715,10 +1733,10 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
@@ -1748,7 +1766,7 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E33" t="s">
         <v>51</v>
@@ -1759,7 +1777,7 @@
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E34" t="s">
         <v>51</v>
@@ -1770,7 +1788,7 @@
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E35" t="s">
         <v>51</v>
@@ -1781,7 +1799,7 @@
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E36" t="s">
         <v>51</v>
@@ -1792,7 +1810,7 @@
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E37" t="s">
         <v>51</v>
@@ -1803,7 +1821,7 @@
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E38" t="s">
         <v>51</v>
@@ -1894,16 +1912,16 @@
         <v>96</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>97</v>
+        <v>155</v>
       </c>
       <c r="E44" t="s">
         <v>96</v>
       </c>
       <c r="F44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G44" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H44" s="18" t="s">
         <v>27</v>
@@ -1911,16 +1929,16 @@
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C45" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G45" t="s">
         <v>84</v>
@@ -1929,21 +1947,21 @@
         <v>27</v>
       </c>
       <c r="I45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C46" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D46" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G46" t="s">
         <v>84</v>
@@ -1952,67 +1970,67 @@
         <v>27</v>
       </c>
       <c r="I46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C47" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D47" t="s">
+        <v>109</v>
+      </c>
+      <c r="E47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F47" t="s">
+        <v>120</v>
+      </c>
+      <c r="G47" t="s">
         <v>110</v>
-      </c>
-      <c r="E47" t="s">
-        <v>113</v>
-      </c>
-      <c r="F47" t="s">
-        <v>121</v>
-      </c>
-      <c r="G47" t="s">
-        <v>111</v>
       </c>
       <c r="H47" t="s">
         <v>27</v>
       </c>
       <c r="I47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C48" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D48" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="E48" t="s">
+        <v>113</v>
+      </c>
+      <c r="F48" t="s">
+        <v>121</v>
+      </c>
+      <c r="G48" t="s">
         <v>117</v>
-      </c>
-      <c r="E48" t="s">
-        <v>114</v>
-      </c>
-      <c r="F48" t="s">
-        <v>122</v>
-      </c>
-      <c r="G48" t="s">
-        <v>118</v>
       </c>
       <c r="H48" t="s">
         <v>27</v>
       </c>
       <c r="I48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C49" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D49" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E49" t="s">
+        <v>123</v>
+      </c>
+      <c r="F49" t="s">
         <v>126</v>
-      </c>
-      <c r="E49" t="s">
-        <v>124</v>
-      </c>
-      <c r="F49" t="s">
-        <v>127</v>
       </c>
       <c r="G49" t="s">
         <v>84</v>
@@ -2021,21 +2039,21 @@
         <v>27</v>
       </c>
       <c r="I49" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C50" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D50" s="33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G50" t="s">
         <v>84</v>
@@ -2044,50 +2062,50 @@
         <v>27</v>
       </c>
       <c r="I50" s="46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="C51" s="32" t="s">
+      <c r="D51" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="E51" t="s">
+        <v>134</v>
+      </c>
+      <c r="F51" t="s">
         <v>135</v>
       </c>
-      <c r="D51" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="E51" t="s">
-        <v>135</v>
-      </c>
-      <c r="F51" t="s">
-        <v>136</v>
-      </c>
       <c r="G51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H51" t="s">
         <v>27</v>
       </c>
       <c r="I51" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C52" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="D52" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="D52" s="33" t="s">
-        <v>153</v>
-      </c>
       <c r="E52" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G52" t="s">
         <v>84</v>
@@ -2096,38 +2114,72 @@
         <v>27</v>
       </c>
     </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C53" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="D53" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="E53" t="s">
+        <v>153</v>
+      </c>
+      <c r="F53" t="s">
+        <v>157</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="H53" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="23" t="s">
+      <c r="C54" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="D54" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="E54" t="s">
+        <v>154</v>
+      </c>
+      <c r="F54" t="s">
+        <v>159</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="H54" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B56" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="25"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="24"/>
+      <c r="H56" s="25"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C56" s="32" t="s">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C58" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D56" s="38" t="s">
+      <c r="D58" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E58" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D57" s="38"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D58" s="38"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D59" s="38"/>
@@ -2138,39 +2190,45 @@
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D61" s="38"/>
     </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D62" s="38"/>
+    </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B63" s="23" t="s">
+      <c r="D63" s="38"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B65" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="24"/>
-      <c r="H63" s="25"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C64" t="s">
+      <c r="C65" s="24"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="24"/>
+      <c r="H65" s="25"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D65" s="38"/>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D66" s="38"/>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D67" s="38"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D68" s="38"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D69" s="38"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D70" s="38"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D71" s="38"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D72" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added carbon footprint parameters
</commit_message>
<xml_diff>
--- a/data/ODYM_Config_Al_cars.xlsx
+++ b/data/ODYM_Config_Al_cars.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450A66F5-852F-4194-BB50-4F3D4BB97AE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E1062B-4B7A-4D1C-954E-D0B215AEB31D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="844" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="165">
   <si>
     <t>Description</t>
   </si>
@@ -511,6 +511,21 @@
   </si>
   <si>
     <t>Srsc</t>
+  </si>
+  <si>
+    <t>Carbon footprint of primary aluminium production</t>
+  </si>
+  <si>
+    <t>Carbon_Footprint_Primary</t>
+  </si>
+  <si>
+    <t>Carbon_Footprint_Secondary</t>
+  </si>
+  <si>
+    <t>Carbon footprint of secondary aluminium production</t>
+  </si>
+  <si>
+    <t>tS</t>
   </si>
 </sst>
 </file>
@@ -680,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -772,6 +787,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1058,14 +1075,14 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="34" t="s">
         <v>34</v>
       </c>
@@ -1073,7 +1090,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="10" t="s">
         <v>35</v>
@@ -1084,14 +1101,14 @@
       </c>
       <c r="G2" s="18"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="10"/>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
       <c r="G3" s="18"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="11" t="s">
         <v>2</v>
@@ -1102,7 +1119,7 @@
       </c>
       <c r="G4" s="42"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="11" t="s">
         <v>49</v>
@@ -1116,133 +1133,133 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="12"/>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="11"/>
       <c r="C7" s="5"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="11"/>
       <c r="C8" s="5"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="14"/>
       <c r="C9" s="5"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="15"/>
       <c r="C11" s="19"/>
       <c r="D11" s="15"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="15"/>
       <c r="C12" s="20"/>
       <c r="D12" s="15"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="15"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
       <c r="D18" s="16"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
       <c r="D23" s="16"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="1"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2"/>
@@ -1255,25 +1272,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:K72"/>
+  <dimension ref="A2:K74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.77734375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.6640625" customWidth="1"/>
-    <col min="6" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
         <v>3</v>
       </c>
@@ -1284,7 +1301,7 @@
       <c r="G2" s="24"/>
       <c r="H2" s="25"/>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C3" s="28" t="s">
         <v>23</v>
       </c>
@@ -1299,7 +1316,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>4</v>
       </c>
@@ -1310,7 +1327,7 @@
       <c r="J4" s="18"/>
       <c r="K4" s="18"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1338,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="18"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>5</v>
       </c>
@@ -1332,13 +1349,13 @@
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D7" s="9"/>
       <c r="I7" s="18"/>
       <c r="J7" s="17"/>
       <c r="K7" s="18"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>36</v>
       </c>
@@ -1352,7 +1369,7 @@
       <c r="J8" s="17"/>
       <c r="K8" s="18"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C9" s="28" t="s">
         <v>23</v>
       </c>
@@ -1369,7 +1386,7 @@
       <c r="J9" s="17"/>
       <c r="K9" s="18"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>6</v>
       </c>
@@ -1380,7 +1397,7 @@
       <c r="J10" s="17"/>
       <c r="K10" s="18"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>53</v>
       </c>
@@ -1391,7 +1408,7 @@
       <c r="J11" s="17"/>
       <c r="K11" s="18"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>54</v>
       </c>
@@ -1402,12 +1419,12 @@
       <c r="J12" s="17"/>
       <c r="K12" s="18"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="I13" s="18"/>
       <c r="J13" s="22"/>
       <c r="K13" s="18"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
         <v>47</v>
       </c>
@@ -1423,7 +1440,7 @@
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C15" s="29" t="s">
         <v>7</v>
       </c>
@@ -1450,7 +1467,7 @@
       </c>
       <c r="K15" s="18"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C16" s="30" t="s">
         <v>11</v>
       </c>
@@ -1475,7 +1492,7 @@
       <c r="J16" s="18"/>
       <c r="K16" s="18"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C17" s="30" t="s">
         <v>60</v>
       </c>
@@ -1500,7 +1517,7 @@
       <c r="J17" s="18"/>
       <c r="K17" s="18"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C18" s="30" t="s">
         <v>12</v>
       </c>
@@ -1525,7 +1542,7 @@
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C19" s="30" t="s">
         <v>13</v>
       </c>
@@ -1550,7 +1567,7 @@
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C20" s="30" t="s">
         <v>66</v>
       </c>
@@ -1575,7 +1592,7 @@
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C21" s="30" t="s">
         <v>93</v>
       </c>
@@ -1598,7 +1615,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C22" s="26" t="s">
         <v>94</v>
       </c>
@@ -1621,7 +1638,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C23" s="26" t="s">
         <v>122</v>
       </c>
@@ -1644,7 +1661,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C24" s="26" t="s">
         <v>128</v>
       </c>
@@ -1667,7 +1684,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C25" s="26" t="s">
         <v>141</v>
       </c>
@@ -1690,7 +1707,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="23" t="s">
         <v>42</v>
       </c>
@@ -1701,7 +1718,7 @@
       <c r="G27" s="24"/>
       <c r="H27" s="25"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C28" s="31" t="s">
         <v>43</v>
       </c>
@@ -1717,7 +1734,7 @@
       <c r="G28" s="35"/>
       <c r="H28" s="35"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C29" s="36">
         <v>0</v>
       </c>
@@ -1728,7 +1745,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C30" s="36">
         <v>1</v>
       </c>
@@ -1739,7 +1756,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C31" s="32">
         <v>2</v>
       </c>
@@ -1750,7 +1767,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C32" s="32">
         <v>3</v>
       </c>
@@ -1761,7 +1778,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C33" s="32">
         <v>4</v>
       </c>
@@ -1772,7 +1789,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C34" s="32">
         <v>5</v>
       </c>
@@ -1783,7 +1800,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C35" s="32">
         <v>6</v>
       </c>
@@ -1794,7 +1811,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C36" s="32">
         <v>7</v>
       </c>
@@ -1805,7 +1822,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C37" s="32">
         <v>8</v>
       </c>
@@ -1816,7 +1833,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C38" s="32">
         <v>9</v>
       </c>
@@ -1827,7 +1844,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="23" t="s">
         <v>21</v>
       </c>
@@ -1838,7 +1855,7 @@
       <c r="G40" s="24"/>
       <c r="H40" s="25"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C41" s="31" t="s">
         <v>24</v>
       </c>
@@ -1861,7 +1878,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C42" s="32" t="s">
         <v>76</v>
       </c>
@@ -1884,7 +1901,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C43" s="32" t="s">
         <v>75</v>
       </c>
@@ -1907,7 +1924,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C44" s="32" t="s">
         <v>96</v>
       </c>
@@ -1927,7 +1944,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C45" s="32" t="s">
         <v>105</v>
       </c>
@@ -1950,7 +1967,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C46" s="32" t="s">
         <v>106</v>
       </c>
@@ -1973,7 +1990,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C47" s="32" t="s">
         <v>112</v>
       </c>
@@ -1996,7 +2013,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C48" s="32" t="s">
         <v>113</v>
       </c>
@@ -2019,7 +2036,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C49" s="32" t="s">
         <v>123</v>
       </c>
@@ -2042,7 +2059,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C50" s="32" t="s">
         <v>137</v>
       </c>
@@ -2065,7 +2082,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>133</v>
       </c>
@@ -2091,7 +2108,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>133</v>
       </c>
@@ -2114,7 +2131,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C53" s="32" t="s">
         <v>153</v>
       </c>
@@ -2134,7 +2151,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C54" s="32" t="s">
         <v>154</v>
       </c>
@@ -2154,81 +2171,121 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B56" s="23" t="s">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C55" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="D55" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="E55" t="s">
+        <v>161</v>
+      </c>
+      <c r="F55" t="s">
+        <v>164</v>
+      </c>
+      <c r="G55" t="s">
+        <v>84</v>
+      </c>
+      <c r="H55" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C56" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="D56" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="E56" t="s">
+        <v>162</v>
+      </c>
+      <c r="F56" t="s">
+        <v>164</v>
+      </c>
+      <c r="G56" t="s">
+        <v>84</v>
+      </c>
+      <c r="H56" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C56" s="24"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="24"/>
-      <c r="H56" s="25"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="25"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C58" s="32" t="s">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C60" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D58" s="38" t="s">
+      <c r="D60" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E60" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D59" s="38"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D60" s="38"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D61" s="38"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D62" s="38"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D63" s="38"/>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B65" s="23" t="s">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D64" s="38"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D65" s="38"/>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C65" s="24"/>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24"/>
-      <c r="G65" s="24"/>
-      <c r="H65" s="25"/>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C66" t="s">
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="25"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D67" s="38"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D68" s="38"/>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D69" s="38"/>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D70" s="38"/>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D71" s="38"/>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D72" s="38"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D73" s="38"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D74" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added class for data prep
Added class for data prep
</commit_message>
<xml_diff>
--- a/data/ODYM_Config_Al_cars.xlsx
+++ b/data/ODYM_Config_Al_cars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E1062B-4B7A-4D1C-954E-D0B215AEB31D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5854143C-FF00-49D1-A6EF-CA8E73FC79AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="844" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="166">
   <si>
     <t>Description</t>
   </si>
@@ -526,6 +526,9 @@
   </si>
   <si>
     <t>tS</t>
+  </si>
+  <si>
+    <t>End of file</t>
   </si>
 </sst>
 </file>
@@ -1272,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:K74"/>
+  <dimension ref="A2:K69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2270,22 +2273,15 @@
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D69" s="38"/>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D70" s="38"/>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D71" s="38"/>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D72" s="38"/>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D73" s="38"/>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D74" s="38"/>
+      <c r="B69" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="24"/>
+      <c r="H69" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated data prep and SP_Coeff
</commit_message>
<xml_diff>
--- a/data/ODYM_Config_Al_cars.xlsx
+++ b/data/ODYM_Config_Al_cars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5854143C-FF00-49D1-A6EF-CA8E73FC79AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA536A1A-B893-4ABD-B0A6-85B5671C66D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="844" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Config" sheetId="5" r:id="rId1"/>
     <sheet name="Setting_Al_cars" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="169">
   <si>
     <t>Description</t>
   </si>
@@ -529,6 +529,15 @@
   </si>
   <si>
     <t>End of file</t>
+  </si>
+  <si>
+    <t>SP_Coeff</t>
+  </si>
+  <si>
+    <t>Correction coefficient to segment split by powertrain</t>
+  </si>
+  <si>
+    <t>sp</t>
   </si>
 </sst>
 </file>
@@ -1275,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:K69"/>
+  <dimension ref="A2:K70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,35 +2223,52 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="23" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C57" s="47" t="s">
+        <v>166</v>
+      </c>
+      <c r="D57" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="E57" t="s">
+        <v>166</v>
+      </c>
+      <c r="F57" t="s">
+        <v>168</v>
+      </c>
+      <c r="G57" t="s">
+        <v>84</v>
+      </c>
+      <c r="H57" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C58" s="24"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="25"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="24"/>
+      <c r="H59" s="25"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C60" s="32" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C61" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D60" s="38" t="s">
+      <c r="D61" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E61" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D61" s="38"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D62" s="38"/>
@@ -2256,32 +2282,35 @@
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D65" s="38"/>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="23" t="s">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D66" s="38"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="24"/>
-      <c r="G67" s="24"/>
-      <c r="H67" s="25"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="24"/>
+      <c r="H68" s="25"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="23" t="s">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="24"/>
-      <c r="H69" s="25"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="24"/>
+      <c r="H70" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
replaced vehcile stock by data from VpC
</commit_message>
<xml_diff>
--- a/data/ODYM_Config_Al_cars.xlsx
+++ b/data/ODYM_Config_Al_cars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76077AD-E0C1-4604-A355-D4D6C423CE0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F96F62-CD1D-4E67-B793-8C03DC048875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5100" yWindow="3780" windowWidth="24975" windowHeight="12615" tabRatio="844" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="844" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="157">
   <si>
     <t>Description</t>
   </si>
@@ -309,9 +309,6 @@
     <t>Marketing Segments</t>
   </si>
   <si>
-    <t>Powertrain_and_Segment</t>
-  </si>
-  <si>
     <t>p</t>
   </si>
   <si>
@@ -321,9 +318,6 @@
     <t>s</t>
   </si>
   <si>
-    <t>rpsc</t>
-  </si>
-  <si>
     <t>Influence of marketing segment on Al content</t>
   </si>
   <si>
@@ -463,9 +457,6 @@
   </si>
   <si>
     <t>Segments</t>
-  </si>
-  <si>
-    <t>Powertrain and Marketing segment by cohort and region</t>
   </si>
   <si>
     <t>Powertrain split by cohort and region</t>
@@ -1257,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:K70"/>
+  <dimension ref="A2:K69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1585,7 @@
         <v>20</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I21" t="s">
         <v>88</v>
@@ -1617,79 +1608,79 @@
         <v>20</v>
       </c>
       <c r="H22" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C23" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E23" t="s">
         <v>87</v>
       </c>
       <c r="F23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G23" t="s">
         <v>20</v>
       </c>
       <c r="H23" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I23" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C24" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D24" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E24" t="s">
         <v>87</v>
       </c>
       <c r="F24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G24" t="s">
         <v>20</v>
       </c>
       <c r="H24" s="26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C25" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" t="s">
+        <v>128</v>
+      </c>
+      <c r="F25" t="s">
+        <v>128</v>
+      </c>
+      <c r="G25" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="H25" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="E25" t="s">
-        <v>130</v>
-      </c>
-      <c r="F25" t="s">
-        <v>130</v>
-      </c>
-      <c r="G25" t="s">
-        <v>132</v>
-      </c>
-      <c r="H25" s="26" t="s">
-        <v>133</v>
-      </c>
       <c r="I25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -1735,10 +1726,10 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
@@ -1768,7 +1759,7 @@
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E33" t="s">
         <v>51</v>
@@ -1779,7 +1770,7 @@
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E34" t="s">
         <v>51</v>
@@ -1790,7 +1781,7 @@
         <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E35" t="s">
         <v>51</v>
@@ -1801,7 +1792,7 @@
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E36" t="s">
         <v>51</v>
@@ -1812,7 +1803,7 @@
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E37" t="s">
         <v>51</v>
@@ -1823,7 +1814,7 @@
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E38" t="s">
         <v>51</v>
@@ -1888,16 +1879,16 @@
         <v>72</v>
       </c>
       <c r="D43" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E43" t="s">
         <v>85</v>
       </c>
       <c r="F43" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H43" t="s">
         <v>27</v>
@@ -1905,36 +1896,36 @@
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C44" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="38" t="s">
-        <v>144</v>
+        <v>97</v>
+      </c>
+      <c r="D44" t="s">
+        <v>96</v>
       </c>
       <c r="E44" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F44" t="s">
-        <v>96</v>
-      </c>
-      <c r="G44" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="H44" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="G44" t="s">
+        <v>80</v>
+      </c>
+      <c r="H44" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C45" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" t="s">
         <v>98</v>
       </c>
+      <c r="D45" s="38" t="s">
+        <v>95</v>
+      </c>
       <c r="E45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G45" t="s">
         <v>80</v>
@@ -1945,19 +1936,19 @@
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C46" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D46" s="38" t="s">
-        <v>97</v>
+        <v>103</v>
+      </c>
+      <c r="D46" t="s">
+        <v>101</v>
       </c>
       <c r="E46" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F46" t="s">
+        <v>110</v>
+      </c>
+      <c r="G46" t="s">
         <v>102</v>
-      </c>
-      <c r="G46" t="s">
-        <v>80</v>
       </c>
       <c r="H46" t="s">
         <v>27</v>
@@ -1965,19 +1956,19 @@
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C47" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="D47" t="s">
-        <v>103</v>
+        <v>104</v>
+      </c>
+      <c r="D47" s="33" t="s">
+        <v>107</v>
       </c>
       <c r="E47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G47" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="H47" t="s">
         <v>27</v>
@@ -1985,19 +1976,19 @@
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C48" s="32" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D48" s="33" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E48" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="F48" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G48" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="H48" t="s">
         <v>27</v>
@@ -2005,16 +1996,16 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C49" s="32" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="D49" s="33" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="E49" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="F49" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="G49" t="s">
         <v>80</v>
@@ -2022,109 +2013,109 @@
       <c r="H49" t="s">
         <v>27</v>
       </c>
+      <c r="I49" s="46"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>122</v>
+      </c>
       <c r="C50" s="32" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D50" s="33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E50" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F50" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="G50" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="H50" t="s">
         <v>27</v>
       </c>
-      <c r="I50" s="46"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="D51" s="33" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="E51" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="F51" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="G51" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="H51" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>124</v>
-      </c>
       <c r="C52" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="D52" s="33" t="s">
-        <v>141</v>
+      <c r="D52" s="38" t="s">
+        <v>142</v>
       </c>
       <c r="E52" t="s">
         <v>140</v>
       </c>
       <c r="F52" t="s">
-        <v>111</v>
-      </c>
-      <c r="G52" t="s">
-        <v>80</v>
-      </c>
-      <c r="H52" t="s">
+        <v>143</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="H52" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C53" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D53" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="E53" t="s">
+        <v>141</v>
+      </c>
+      <c r="F53" t="s">
         <v>145</v>
       </c>
-      <c r="E53" t="s">
-        <v>142</v>
-      </c>
-      <c r="F53" t="s">
-        <v>146</v>
-      </c>
       <c r="G53" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H53" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C54" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="D54" s="38" t="s">
+      <c r="C54" s="47" t="s">
         <v>147</v>
       </c>
+      <c r="D54" s="48" t="s">
+        <v>146</v>
+      </c>
       <c r="E54" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="F54" t="s">
-        <v>148</v>
-      </c>
-      <c r="G54" s="18" t="s">
-        <v>94</v>
+        <v>150</v>
+      </c>
+      <c r="G54" t="s">
+        <v>80</v>
       </c>
       <c r="H54" s="18" t="s">
         <v>27</v>
@@ -2132,16 +2123,16 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C55" s="47" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D55" s="48" t="s">
         <v>149</v>
       </c>
       <c r="E55" t="s">
+        <v>148</v>
+      </c>
+      <c r="F55" t="s">
         <v>150</v>
-      </c>
-      <c r="F55" t="s">
-        <v>153</v>
       </c>
       <c r="G55" t="s">
         <v>80</v>
@@ -2152,70 +2143,53 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C56" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="D56" s="48" t="s">
         <v>152</v>
       </c>
+      <c r="D56" s="33" t="s">
+        <v>153</v>
+      </c>
       <c r="E56" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F56" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G56" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="H56" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C57" s="47" t="s">
-        <v>155</v>
-      </c>
-      <c r="D57" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="E57" t="s">
-        <v>155</v>
-      </c>
-      <c r="F57" t="s">
-        <v>157</v>
-      </c>
-      <c r="G57" t="s">
-        <v>104</v>
-      </c>
-      <c r="H57" s="18" t="s">
-        <v>27</v>
-      </c>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="25"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="24"/>
-      <c r="H59" s="25"/>
+      <c r="C59" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
-        <v>38</v>
+      <c r="C60" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D60" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C61" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="D61" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="E61" t="s">
-        <v>41</v>
-      </c>
+      <c r="D61" s="38"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D62" s="38"/>
@@ -2229,35 +2203,32 @@
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D65" s="38"/>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D66" s="38"/>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="25"/>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-      <c r="F68" s="24"/>
-      <c r="G68" s="24"/>
-      <c r="H68" s="25"/>
+      <c r="C68" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24"/>
-      <c r="G70" s="24"/>
-      <c r="H70" s="25"/>
+      <c r="B69" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="24"/>
+      <c r="H69" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated paramters and config files for individual scenarios
</commit_message>
<xml_diff>
--- a/data/ODYM_Config_Al_cars.xlsx
+++ b/data/ODYM_Config_Al_cars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F96F62-CD1D-4E67-B793-8C03DC048875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27303B2B-B18F-4BD3-A0F8-5361A1C9FDD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="844" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-315" windowWidth="38640" windowHeight="21240" tabRatio="844" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="183">
   <si>
     <t>Description</t>
   </si>
@@ -363,9 +363,6 @@
     <t>tr</t>
   </si>
   <si>
-    <t>erc</t>
-  </si>
-  <si>
     <t>crpsz</t>
   </si>
   <si>
@@ -420,9 +417,6 @@
     <t>Scenario</t>
   </si>
   <si>
-    <t>Scenarios considered</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
@@ -462,9 +456,6 @@
     <t>Powertrain split by cohort and region</t>
   </si>
   <si>
-    <t>Srpc</t>
-  </si>
-  <si>
     <t xml:space="preserve">Segment split by cohort and region </t>
   </si>
   <si>
@@ -483,9 +474,6 @@
     <t>Carbon footprint of secondary aluminium production</t>
   </si>
   <si>
-    <t>tS</t>
-  </si>
-  <si>
     <t>End of file</t>
   </si>
   <si>
@@ -498,10 +486,100 @@
     <t>psc</t>
   </si>
   <si>
-    <t>Srt</t>
-  </si>
-  <si>
     <t>Vehicle stock per region</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Population per world region</t>
+  </si>
+  <si>
+    <t>Ptr</t>
+  </si>
+  <si>
+    <t>Population_Scenario</t>
+  </si>
+  <si>
+    <t>Scenario for population</t>
+  </si>
+  <si>
+    <t>pop_scen</t>
+  </si>
+  <si>
+    <t>Vtr</t>
+  </si>
+  <si>
+    <t>Vehicle_Ownership_Scenario</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>ownership_scen</t>
+  </si>
+  <si>
+    <t>Scenario for vehicle ownership per capita</t>
+  </si>
+  <si>
+    <t>Vehicle ownership per capita (cars/1000 cap)</t>
+  </si>
+  <si>
+    <t>Vehicle_Ownership</t>
+  </si>
+  <si>
+    <t>Powertrain_Scenario</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>powertrain_scen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenario for powertrain type split </t>
+  </si>
+  <si>
+    <t>Segment_Scenario</t>
+  </si>
+  <si>
+    <t>Scenario for segment split</t>
+  </si>
+  <si>
+    <t>segment_scen</t>
+  </si>
+  <si>
+    <t>Al_Content_Scenario</t>
+  </si>
+  <si>
+    <t>Scenarios for average Al content</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>al_scen</t>
+  </si>
+  <si>
+    <t>Trpc</t>
+  </si>
+  <si>
+    <t>Aerc</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>scen</t>
+  </si>
+  <si>
+    <t>Zrt</t>
+  </si>
+  <si>
+    <t>tZ</t>
   </si>
 </sst>
 </file>
@@ -1248,10 +1326,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:K69"/>
+  <dimension ref="A2:K76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D44" sqref="A44:XFD44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,12 +1689,12 @@
         <v>94</v>
       </c>
       <c r="I22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C23" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D23" s="38" t="s">
         <v>105</v>
@@ -1625,7 +1703,7 @@
         <v>87</v>
       </c>
       <c r="F23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G23" t="s">
         <v>20</v>
@@ -1634,165 +1712,225 @@
         <v>106</v>
       </c>
       <c r="I23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C24" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="38" t="s">
         <v>117</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>118</v>
       </c>
       <c r="E24" t="s">
         <v>87</v>
       </c>
       <c r="F24" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G24" t="s">
         <v>20</v>
       </c>
       <c r="H24" s="26" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C25" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" t="s">
+        <v>156</v>
+      </c>
+      <c r="G25" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="I25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="D26" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="E26" t="s">
+        <v>127</v>
+      </c>
+      <c r="F26" t="s">
+        <v>160</v>
+      </c>
+      <c r="G26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="I26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="E27" t="s">
+        <v>127</v>
+      </c>
+      <c r="F27" t="s">
+        <v>166</v>
+      </c>
+      <c r="G27" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="I27" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C28" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="E28" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" t="s">
+        <v>170</v>
+      </c>
+      <c r="G28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="I28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C29" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="E29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F29" t="s">
+        <v>173</v>
+      </c>
+      <c r="G29" t="s">
         <v>128</v>
       </c>
-      <c r="D25" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="H29" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="I29" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="E30" t="s">
+        <v>127</v>
+      </c>
+      <c r="F30" t="s">
+        <v>127</v>
+      </c>
+      <c r="G30" t="s">
         <v>128</v>
       </c>
-      <c r="F25" t="s">
-        <v>128</v>
-      </c>
-      <c r="G25" t="s">
-        <v>130</v>
-      </c>
-      <c r="H25" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="I25" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="23" t="s">
+      <c r="H30" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="I30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="25"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C28" s="31" t="s">
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="25"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D33" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E33" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="28" t="s">
+      <c r="F33" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C29" s="36">
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="36">
         <v>0</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D34" t="s">
         <v>70</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C30" s="36">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C35" s="36">
         <v>1</v>
       </c>
-      <c r="D30" t="s">
-        <v>137</v>
-      </c>
-      <c r="E30" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C31" s="32">
-        <v>2</v>
-      </c>
-      <c r="D31" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C32" s="32">
-        <v>3</v>
-      </c>
-      <c r="D32" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C33" s="32">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
-        <v>125</v>
-      </c>
-      <c r="E33" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C34" s="32">
-        <v>5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>123</v>
-      </c>
-      <c r="E34" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C35" s="32">
-        <v>6</v>
-      </c>
       <c r="D35" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E35" t="s">
-        <v>51</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C36" s="32">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>133</v>
+        <v>71</v>
       </c>
       <c r="E36" t="s">
         <v>51</v>
@@ -1800,10 +1938,10 @@
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C37" s="32">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>134</v>
+        <v>30</v>
       </c>
       <c r="E37" t="s">
         <v>51</v>
@@ -1811,201 +1949,158 @@
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C38" s="32">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E38" t="s">
         <v>51</v>
       </c>
     </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C39" s="32">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>122</v>
+      </c>
+      <c r="E39" t="s">
+        <v>51</v>
+      </c>
+    </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="s">
+      <c r="C40" s="32">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>130</v>
+      </c>
+      <c r="E40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="32">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>131</v>
+      </c>
+      <c r="E41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C42" s="32">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C43" s="32">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="25"/>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C41" s="31" t="s">
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="25"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C46" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="28" t="s">
+      <c r="D46" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E41" s="28" t="s">
+      <c r="E46" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="F41" s="28" t="s">
+      <c r="F46" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G41" s="28" t="s">
+      <c r="G46" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="H41" s="28" t="s">
+      <c r="H46" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="I41" s="43" t="s">
+      <c r="I46" s="43" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C42" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="D42" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="E42" t="s">
-        <v>84</v>
-      </c>
-      <c r="F42" t="s">
-        <v>81</v>
-      </c>
-      <c r="G42" t="s">
-        <v>80</v>
-      </c>
-      <c r="H42" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C43" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" t="s">
-        <v>156</v>
-      </c>
-      <c r="E43" t="s">
-        <v>85</v>
-      </c>
-      <c r="F43" t="s">
-        <v>155</v>
-      </c>
-      <c r="G43" t="s">
-        <v>102</v>
-      </c>
-      <c r="H43" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C44" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="D44" t="s">
-        <v>96</v>
-      </c>
-      <c r="E44" t="s">
-        <v>97</v>
-      </c>
-      <c r="F44" t="s">
-        <v>99</v>
-      </c>
-      <c r="G44" t="s">
-        <v>80</v>
-      </c>
-      <c r="H44" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C45" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="E45" t="s">
-        <v>98</v>
-      </c>
-      <c r="F45" t="s">
-        <v>100</v>
-      </c>
-      <c r="G45" t="s">
-        <v>80</v>
-      </c>
-      <c r="H45" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C46" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D46" t="s">
-        <v>101</v>
-      </c>
-      <c r="E46" t="s">
-        <v>103</v>
-      </c>
-      <c r="F46" t="s">
-        <v>110</v>
-      </c>
-      <c r="G46" t="s">
-        <v>102</v>
-      </c>
-      <c r="H46" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C47" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="D47" s="33" t="s">
-        <v>107</v>
+        <v>153</v>
+      </c>
+      <c r="D47" s="38" t="s">
+        <v>154</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>153</v>
       </c>
       <c r="F47" t="s">
-        <v>111</v>
+        <v>155</v>
       </c>
       <c r="G47" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H47" t="s">
         <v>27</v>
       </c>
+      <c r="I47" s="41"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C48" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="D48" s="33" t="s">
-        <v>115</v>
+        <v>165</v>
+      </c>
+      <c r="D48" s="38" t="s">
+        <v>164</v>
       </c>
       <c r="E48" t="s">
-        <v>113</v>
+        <v>165</v>
       </c>
       <c r="F48" t="s">
-        <v>116</v>
+        <v>159</v>
       </c>
       <c r="G48" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="H48" t="s">
         <v>27</v>
       </c>
+      <c r="I48" s="41"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C49" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="D49" s="33" t="s">
-        <v>127</v>
+        <v>73</v>
+      </c>
+      <c r="D49" s="38" t="s">
+        <v>69</v>
       </c>
       <c r="E49" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="F49" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="G49" t="s">
         <v>80</v>
@@ -2013,23 +2108,19 @@
       <c r="H49" t="s">
         <v>27</v>
       </c>
-      <c r="I49" s="46"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>122</v>
-      </c>
       <c r="C50" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="D50" s="33" t="s">
-        <v>126</v>
+        <v>72</v>
+      </c>
+      <c r="D50" t="s">
+        <v>151</v>
       </c>
       <c r="E50" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="F50" t="s">
-        <v>124</v>
+        <v>181</v>
       </c>
       <c r="G50" t="s">
         <v>102</v>
@@ -2039,20 +2130,17 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>122</v>
-      </c>
       <c r="C51" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="D51" s="33" t="s">
-        <v>139</v>
+        <v>97</v>
+      </c>
+      <c r="D51" t="s">
+        <v>96</v>
       </c>
       <c r="E51" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="F51" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="G51" t="s">
         <v>80</v>
@@ -2063,172 +2151,319 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C52" s="32" t="s">
-        <v>140</v>
+        <v>98</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="E52" t="s">
-        <v>140</v>
+        <v>98</v>
       </c>
       <c r="F52" t="s">
-        <v>143</v>
-      </c>
-      <c r="G52" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="H52" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="G52" t="s">
+        <v>80</v>
+      </c>
+      <c r="H52" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C53" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="D53" s="38" t="s">
-        <v>144</v>
+        <v>103</v>
+      </c>
+      <c r="D53" t="s">
+        <v>101</v>
       </c>
       <c r="E53" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="F53" t="s">
-        <v>145</v>
-      </c>
-      <c r="G53" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="G53" t="s">
         <v>93</v>
       </c>
-      <c r="H53" s="18" t="s">
+      <c r="H53" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C54" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="D54" s="48" t="s">
-        <v>146</v>
+      <c r="C54" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="33" t="s">
+        <v>107</v>
       </c>
       <c r="E54" t="s">
-        <v>147</v>
+        <v>104</v>
       </c>
       <c r="F54" t="s">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="G54" t="s">
-        <v>80</v>
-      </c>
-      <c r="H54" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="H54" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C55" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="D55" s="48" t="s">
-        <v>149</v>
+      <c r="C55" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D55" s="33" t="s">
+        <v>114</v>
       </c>
       <c r="E55" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="F55" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="G55" t="s">
         <v>80</v>
       </c>
-      <c r="H55" s="18" t="s">
+      <c r="H55" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C56" s="47" t="s">
-        <v>152</v>
+      <c r="C56" s="32" t="s">
+        <v>124</v>
       </c>
       <c r="D56" s="33" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="E56" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="F56" t="s">
-        <v>154</v>
+        <v>109</v>
       </c>
       <c r="G56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H56" t="s">
+        <v>27</v>
+      </c>
+      <c r="I56" s="46"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>121</v>
+      </c>
+      <c r="C57" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D57" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E57" t="s">
+        <v>122</v>
+      </c>
+      <c r="F57" t="s">
+        <v>123</v>
+      </c>
+      <c r="G57" t="s">
         <v>102</v>
       </c>
-      <c r="H56" s="18" t="s">
+      <c r="H57" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C58" s="24"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="25"/>
+      <c r="A58" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="D58" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="E58" t="s">
+        <v>136</v>
+      </c>
+      <c r="F58" t="s">
+        <v>109</v>
+      </c>
+      <c r="G58" t="s">
+        <v>80</v>
+      </c>
+      <c r="H58" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
-        <v>38</v>
+      <c r="C59" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="D59" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="E59" t="s">
+        <v>138</v>
+      </c>
+      <c r="F59" t="s">
+        <v>177</v>
+      </c>
+      <c r="G59" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="H59" s="18" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C60" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="D60" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="E60" t="s">
+        <v>139</v>
+      </c>
+      <c r="F60" t="s">
+        <v>142</v>
+      </c>
+      <c r="G60" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="H60" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C61" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="D61" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="E61" t="s">
+        <v>144</v>
+      </c>
+      <c r="F61" t="s">
+        <v>182</v>
+      </c>
+      <c r="G61" t="s">
+        <v>80</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C62" s="47" t="s">
+        <v>145</v>
+      </c>
+      <c r="D62" s="48" t="s">
+        <v>146</v>
+      </c>
+      <c r="E62" t="s">
+        <v>145</v>
+      </c>
+      <c r="F62" t="s">
+        <v>182</v>
+      </c>
+      <c r="G62" t="s">
+        <v>80</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C63" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D63" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="E63" t="s">
+        <v>148</v>
+      </c>
+      <c r="F63" t="s">
+        <v>150</v>
+      </c>
+      <c r="G63" t="s">
+        <v>102</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65" s="24"/>
+      <c r="D65" s="24"/>
+      <c r="E65" s="24"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="24"/>
+      <c r="H65" s="25"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C67" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D60" s="38" t="s">
+      <c r="D67" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E67" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D61" s="38"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D62" s="38"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D63" s="38"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D64" s="38"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D65" s="38"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="23" t="s">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D68" s="38"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D69" s="38"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D70" s="38"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D71" s="38"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D72" s="38"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="24"/>
-      <c r="G67" s="24"/>
-      <c r="H67" s="25"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
+      <c r="C74" s="24"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="24"/>
+      <c r="H74" s="25"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="24"/>
-      <c r="H69" s="25"/>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="C76" s="24"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="24"/>
+      <c r="G76" s="24"/>
+      <c r="H76" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>